<commit_message>
fix: bug status dosen management
</commit_message>
<xml_diff>
--- a/public/excel/template_lomba.xlsx
+++ b/public/excel/template_lomba.xlsx
@@ -498,5 +498,14 @@
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: admin kelola data lomba
</commit_message>
<xml_diff>
--- a/public/excel/template_lomba.xlsx
+++ b/public/excel/template_lomba.xlsx
@@ -15,9 +15,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
-  <si>
-    <t>Keahlian ID</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="17">
+  <si>
+    <t>Bidang Keahlian</t>
   </si>
   <si>
     <t>Tingkatan ID</t>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Link Poster</t>
+  </si>
+  <si>
+    <t>Frontend Developer, Backend Developer</t>
   </si>
   <si>
     <t>Lomba Hackathon</t>
@@ -426,7 +429,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.997" bestFit="true" customWidth="true" style="0"/>
+    <col min="1" max="1" width="44.703" bestFit="true" customWidth="true" style="0"/>
     <col min="10" max="10" width="13.997" bestFit="true" customWidth="true" style="0"/>
   </cols>
   <sheetData>
@@ -463,8 +466,8 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -473,39 +476,30 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
-  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
-    <oddHeader/>
-    <oddFooter/>
-    <evenHeader/>
-    <evenFooter/>
-    <firstHeader/>
-    <firstFooter/>
-  </headerFooter>
-  <tableParts count="0"/>
 </worksheet>
 </file>
</xml_diff>